<commit_message>
fix error in excel formula
</commit_message>
<xml_diff>
--- a/courses/excel/accounting_example.xlsx
+++ b/courses/excel/accounting_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Dropbox\jfimbett.github.io\courses\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CF88B6-007B-4C7C-BA43-B30B7D4B689D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF7AF1B-D651-4963-B918-405706C4E69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CBA1142-981A-4A10-B64B-1FE78F4F0EB9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3CBA1142-981A-4A10-B64B-1FE78F4F0EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,7 +568,7 @@
   <dimension ref="D4:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +828,7 @@
         <v>17.324999999999999</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" ref="H12:K12" si="4">I6*(0.1)*0.99</f>
+        <f t="shared" ref="I12:K12" si="4">I6*(0.1)*0.99</f>
         <v>20.79</v>
       </c>
       <c r="J12" s="2">
@@ -1034,24 +1034,24 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f>G19+G17</f>
-        <v>6.4599999999999991</v>
+        <f>G17</f>
+        <v>1.4</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" ref="H20:K20" si="8">H19+H17</f>
-        <v>10.074999999999999</v>
+        <f t="shared" ref="H20:K20" si="8">H17</f>
+        <v>1.4</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="8"/>
-        <v>12.69</v>
+        <v>1.4</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="8"/>
-        <v>15.305</v>
+        <v>1.4</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="8"/>
-        <v>17.919999999999998</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1088,12 +1088,12 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f>G20-G21</f>
+        <f>G20-G21+G19</f>
         <v>66.459999999999994</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" ref="H22:J22" si="9">H20-H21</f>
-        <v>25.074999999999999</v>
+        <f t="shared" ref="H22:K22" si="9">H20-H21+H19</f>
+        <v>25.074999999999996</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="9"/>
@@ -1104,7 +1104,7 @@
         <v>30.305000000000028</v>
       </c>
       <c r="K22" s="2">
-        <f>K20-K21</f>
+        <f t="shared" si="9"/>
         <v>32.919999999999973</v>
       </c>
     </row>

</xml_diff>